<commit_message>
Fix bug in initial vector count
</commit_message>
<xml_diff>
--- a/2021/day14.xlsx
+++ b/2021/day14.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tchan/workspace/advent_of_code/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BDADFD-D684-F94A-BDF3-B86A30BC13B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EF388-45E0-8B43-8694-9AD833D4C697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="660" windowWidth="16380" windowHeight="16840" xr2:uid="{DE175EE8-7C66-EC48-967C-5A43A324EDEA}"/>
+    <workbookView xWindow="17940" yWindow="3780" windowWidth="16380" windowHeight="16840" xr2:uid="{DE175EE8-7C66-EC48-967C-5A43A324EDEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -448,9 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693C373B-4E9D-BE4A-B455-341E85EBBA49}">
   <dimension ref="A2:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>